<commit_message>
Update the speaker list, Olga presentation
</commit_message>
<xml_diff>
--- a/IS Meeting booking grid.xlsx
+++ b/IS Meeting booking grid.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahummel\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahummel\Documents\Presentation\IS Team Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD73EDED-F423-4848-848B-DB8FC2FFE203}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01114BA3-ADE6-4F10-87D5-84AFA9009C0C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="10440" xr2:uid="{CC0DBEE7-A10C-49D3-9C55-599B590CB2DE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>IS Meeting booking grid</t>
   </si>
@@ -52,6 +52,57 @@
   </si>
   <si>
     <t>5 minutes</t>
+  </si>
+  <si>
+    <t>Olga Agady</t>
+  </si>
+  <si>
+    <t>Integration with Box.com</t>
+  </si>
+  <si>
+    <t>Alan Hummel</t>
+  </si>
+  <si>
+    <t>Using Git</t>
+  </si>
+  <si>
+    <t>John Hynes</t>
+  </si>
+  <si>
+    <t>Java member</t>
+  </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>Welcome, team</t>
+  </si>
+  <si>
+    <t>10 minutes</t>
+  </si>
+  <si>
+    <t>Digitalization Team Update</t>
+  </si>
+  <si>
+    <t>VBS</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Senthil/Melissa</t>
+  </si>
+  <si>
+    <t>Shazi</t>
+  </si>
+  <si>
+    <t>UCS Migration Tech Team</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>RA</t>
   </si>
 </sst>
 </file>
@@ -90,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -99,6 +150,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -108,6 +174,120 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -120,7 +300,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -135,7 +315,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -147,12 +327,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,43 +656,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE3006B-BCA9-48F6-BCDD-55DDFA88D9B9}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C8" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update the speaker list, changed order
</commit_message>
<xml_diff>
--- a/IS Meeting booking grid.xlsx
+++ b/IS Meeting booking grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahummel\Documents\Presentation\IS Team Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01114BA3-ADE6-4F10-87D5-84AFA9009C0C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53874FE7-7156-45A3-8A4B-6102D1DC6EE0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="10440" xr2:uid="{CC0DBEE7-A10C-49D3-9C55-599B590CB2DE}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
-  <si>
-    <t>IS Meeting booking grid</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Subject</t>
   </si>
@@ -103,6 +100,18 @@
   </si>
   <si>
     <t>RA</t>
+  </si>
+  <si>
+    <t>Connie Liu</t>
+  </si>
+  <si>
+    <t>Presenting new team member</t>
+  </si>
+  <si>
+    <t>1 minute</t>
+  </si>
+  <si>
+    <t>IS Meeting booking - November 22nd</t>
   </si>
 </sst>
 </file>
@@ -327,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -342,6 +351,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,11 +668,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE3006B-BCA9-48F6-BCDD-55DDFA88D9B9}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -671,122 +681,133 @@
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>15</v>
+      <c r="A6" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>5</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="B12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>6</v>
+      <c r="C13" s="13" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated presentation list. Added Git presentation and Olga header presentation.
</commit_message>
<xml_diff>
--- a/IS Meeting booking grid.xlsx
+++ b/IS Meeting booking grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahummel\Documents\Presentation\IS Team Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53874FE7-7156-45A3-8A4B-6102D1DC6EE0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8F63CA-9AFC-4948-8917-82C33CE9C938}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="10440" xr2:uid="{CC0DBEE7-A10C-49D3-9C55-599B590CB2DE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Subject</t>
   </si>
@@ -112,6 +112,18 @@
   </si>
   <si>
     <t>IS Meeting booking - November 22nd</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>UCS</t>
+  </si>
+  <si>
+    <t>Donovan</t>
+  </si>
+  <si>
+    <t>MFA</t>
   </si>
 </sst>
 </file>
@@ -150,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -332,11 +344,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -354,6 +399,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,9 +718,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE3006B-BCA9-48F6-BCDD-55DDFA88D9B9}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -774,35 +826,57 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B15" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C15" s="13" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated agenda - Sanjay presentation.
</commit_message>
<xml_diff>
--- a/IS Meeting booking grid.xlsx
+++ b/IS Meeting booking grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahummel\Documents\Presentation\IS Team Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9F8284-25F9-4411-8B19-2C65831737AE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8895DAC4-1ECD-4244-9321-262F0CF8D7A8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="10440" xr2:uid="{CC0DBEE7-A10C-49D3-9C55-599B590CB2DE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Subject</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>MFA</t>
+  </si>
+  <si>
+    <t>Sanjay</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -150,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -365,11 +371,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -392,6 +437,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE3006B-BCA9-48F6-BCDD-55DDFA88D9B9}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,14 +883,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B14" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C14" s="13" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update to the Agenda, including Sammy Douglas.
</commit_message>
<xml_diff>
--- a/IS Meeting booking grid.xlsx
+++ b/IS Meeting booking grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahummel\Documents\Presentation\IS Team Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8895DAC4-1ECD-4244-9321-262F0CF8D7A8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B91AF9-0C18-4023-BDC6-A560593D42F7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="10440" xr2:uid="{CC0DBEE7-A10C-49D3-9C55-599B590CB2DE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Subject</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>Sammy Douglas</t>
+  </si>
+  <si>
+    <t>Destruction Update</t>
   </si>
 </sst>
 </file>
@@ -754,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE3006B-BCA9-48F6-BCDD-55DDFA88D9B9}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,56 +858,67 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C12" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B13" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C13" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B14" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C14" s="24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B15" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C15" s="13" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>